<commit_message>
CLUTCH Control Testing 5
refined xClutch map to use all the range (previously was using only half)
</commit_message>
<xml_diff>
--- a/Docs/ClutchMap_v01.xlsx
+++ b/Docs/ClutchMap_v01.xlsx
@@ -210,34 +210,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
+                  <c:v>1100</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1180</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1260</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1340</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1420</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>1500</c:v>
                 </c:pt>
-                <c:pt idx="1">
-                  <c:v>1575</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1650</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1725</c:v>
-                </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="6">
+                  <c:v>1580</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1660</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1720</c:v>
+                </c:pt>
+                <c:pt idx="9">
                   <c:v>1800</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1816</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>1832</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>1848</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>1864</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>1880</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>1900</c:v>
@@ -255,11 +255,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-903469472"/>
-        <c:axId val="-903480352"/>
+        <c:axId val="1955300704"/>
+        <c:axId val="1955295264"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-903469472"/>
+        <c:axId val="1955300704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -316,15 +316,15 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-903480352"/>
+        <c:crossAx val="1955295264"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-903480352"/>
+        <c:axId val="1955295264"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:min val="1450"/>
+          <c:min val="1000"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -379,7 +379,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-903469472"/>
+        <c:crossAx val="1955300704"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1285,7 +1285,7 @@
   <dimension ref="C6:D17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1307,7 +1307,7 @@
         <v>0</v>
       </c>
       <c r="D7">
-        <v>1500</v>
+        <v>1100</v>
       </c>
     </row>
     <row r="8" spans="3:4" x14ac:dyDescent="0.25">
@@ -1315,8 +1315,7 @@
         <v>10</v>
       </c>
       <c r="D8">
-        <f>D7+75</f>
-        <v>1575</v>
+        <v>1180</v>
       </c>
     </row>
     <row r="9" spans="3:4" x14ac:dyDescent="0.25">
@@ -1324,8 +1323,7 @@
         <v>20</v>
       </c>
       <c r="D9">
-        <f t="shared" ref="D9:D10" si="0">D8+75</f>
-        <v>1650</v>
+        <v>1260</v>
       </c>
     </row>
     <row r="10" spans="3:4" x14ac:dyDescent="0.25">
@@ -1333,8 +1331,7 @@
         <v>30</v>
       </c>
       <c r="D10">
-        <f t="shared" si="0"/>
-        <v>1725</v>
+        <v>1340</v>
       </c>
     </row>
     <row r="11" spans="3:4" x14ac:dyDescent="0.25">
@@ -1342,7 +1339,7 @@
         <v>40</v>
       </c>
       <c r="D11">
-        <v>1800</v>
+        <v>1420</v>
       </c>
     </row>
     <row r="12" spans="3:4" x14ac:dyDescent="0.25">
@@ -1350,8 +1347,7 @@
         <v>50</v>
       </c>
       <c r="D12">
-        <f>D11+16</f>
-        <v>1816</v>
+        <v>1500</v>
       </c>
     </row>
     <row r="13" spans="3:4" x14ac:dyDescent="0.25">
@@ -1359,8 +1355,7 @@
         <v>60</v>
       </c>
       <c r="D13">
-        <f t="shared" ref="D13:D15" si="1">D12+16</f>
-        <v>1832</v>
+        <v>1580</v>
       </c>
     </row>
     <row r="14" spans="3:4" x14ac:dyDescent="0.25">
@@ -1368,8 +1363,7 @@
         <v>70</v>
       </c>
       <c r="D14">
-        <f t="shared" si="1"/>
-        <v>1848</v>
+        <v>1660</v>
       </c>
     </row>
     <row r="15" spans="3:4" x14ac:dyDescent="0.25">
@@ -1377,8 +1371,7 @@
         <v>80</v>
       </c>
       <c r="D15">
-        <f t="shared" si="1"/>
-        <v>1864</v>
+        <v>1720</v>
       </c>
     </row>
     <row r="16" spans="3:4" x14ac:dyDescent="0.25">
@@ -1386,8 +1379,7 @@
         <v>90</v>
       </c>
       <c r="D16">
-        <f>D15+16</f>
-        <v>1880</v>
+        <v>1800</v>
       </c>
     </row>
     <row r="17" spans="3:4" x14ac:dyDescent="0.25">

</xml_diff>